<commit_message>
adding ids, running for some data points
</commit_message>
<xml_diff>
--- a/ids stations.xlsx
+++ b/ids stations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\@@ Python\Jaar 5\Q3\ENVM1502\Git\ENVM1502-Catchment-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB216B8-B10E-4FF0-9F77-51AB910D6E02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C507F40A-4993-4845-A11B-52CE60F03A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{37768EAB-540B-4408-BCC7-B7FCBC472778}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="87">
   <si>
     <t>USGS</t>
   </si>
@@ -128,9 +128,6 @@
     <t>HOOSIC RIVER NEAR EAGLE BRIDGE NY</t>
   </si>
   <si>
-    <t>Upper</t>
-  </si>
-  <si>
     <t>Hudson-Hoosic</t>
   </si>
   <si>
@@ -294,6 +291,12 @@
   </si>
   <si>
     <t>CROTON R AT NEW CROTON DAM NR CROTON-ON-HUDSON NY</t>
+  </si>
+  <si>
+    <t>initial</t>
+  </si>
+  <si>
+    <t>Upper hudson</t>
   </si>
 </sst>
 </file>
@@ -648,10 +651,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2E30F5-87A7-4420-9A6F-3C3B0374E5EE}">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B75" activeCellId="5" sqref="B21:B28 B30:B39 B40 B42:B70 B72:B73 B75:B94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,13 +666,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>1312000</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -677,10 +674,10 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>1315500</v>
+        <v>1312000</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -688,10 +685,10 @@
         <v>0</v>
       </c>
       <c r="B3">
-        <v>1318500</v>
+        <v>1315500</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -699,10 +696,10 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>1327750</v>
+        <v>1318500</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -710,10 +707,10 @@
         <v>0</v>
       </c>
       <c r="B5">
-        <v>1328770</v>
+        <v>1327750</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -721,10 +718,10 @@
         <v>0</v>
       </c>
       <c r="B6">
-        <v>1335754</v>
+        <v>1328770</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -732,10 +729,10 @@
         <v>0</v>
       </c>
       <c r="B7">
-        <v>1335755</v>
+        <v>1335754</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -743,10 +740,10 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <v>1358000</v>
+        <v>1335755</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -754,10 +751,10 @@
         <v>0</v>
       </c>
       <c r="B9">
-        <v>1359139</v>
+        <v>1358000</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -765,10 +762,10 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>1359165</v>
+        <v>1359139</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -776,10 +773,10 @@
         <v>0</v>
       </c>
       <c r="B11">
-        <v>135980207</v>
+        <v>1359165</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -787,10 +784,10 @@
         <v>0</v>
       </c>
       <c r="B12">
-        <v>1372043</v>
+        <v>135980207</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -798,10 +795,10 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>1372058</v>
+        <v>1372043</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -809,10 +806,10 @@
         <v>0</v>
       </c>
       <c r="B14">
-        <v>1374019</v>
+        <v>1372058</v>
       </c>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -820,10 +817,10 @@
         <v>0</v>
       </c>
       <c r="B15">
-        <v>1376269</v>
+        <v>1374019</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -831,10 +828,10 @@
         <v>0</v>
       </c>
       <c r="B16">
-        <v>1376307</v>
+        <v>1376269</v>
       </c>
       <c r="C16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -842,10 +839,10 @@
         <v>0</v>
       </c>
       <c r="B17">
-        <v>1376515</v>
+        <v>1376307</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -853,39 +850,39 @@
         <v>0</v>
       </c>
       <c r="B18">
+        <v>1376515</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
         <v>1376520</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-    </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>131199050</v>
-      </c>
-      <c r="C20" t="s">
-        <v>19</v>
-      </c>
+      <c r="A20" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>0</v>
       </c>
       <c r="B21">
-        <v>1312000</v>
+        <v>131199050</v>
       </c>
       <c r="C21" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -893,10 +890,10 @@
         <v>0</v>
       </c>
       <c r="B22">
-        <v>1315000</v>
+        <v>1312000</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -904,10 +901,10 @@
         <v>0</v>
       </c>
       <c r="B23">
-        <v>1315170</v>
+        <v>1315000</v>
       </c>
       <c r="C23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -915,10 +912,10 @@
         <v>0</v>
       </c>
       <c r="B24">
-        <v>1315226</v>
+        <v>1315170</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -926,10 +923,10 @@
         <v>0</v>
       </c>
       <c r="B25">
-        <v>1315227</v>
+        <v>1315226</v>
       </c>
       <c r="C25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -937,10 +934,10 @@
         <v>0</v>
       </c>
       <c r="B26">
-        <v>1315500</v>
+        <v>1315227</v>
       </c>
       <c r="C26" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -948,39 +945,39 @@
         <v>0</v>
       </c>
       <c r="B27">
+        <v>1315500</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
         <v>1318500</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C28" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-    </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29">
-        <v>1327500</v>
-      </c>
-      <c r="C29" t="s">
-        <v>24</v>
-      </c>
+      <c r="A29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>0</v>
       </c>
       <c r="B30">
-        <v>1327750</v>
+        <v>1327500</v>
       </c>
       <c r="C30" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -988,10 +985,10 @@
         <v>0</v>
       </c>
       <c r="B31">
-        <v>1328770</v>
+        <v>1327750</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -999,10 +996,10 @@
         <v>0</v>
       </c>
       <c r="B32">
-        <v>1329490</v>
+        <v>1328770</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1010,10 +1007,10 @@
         <v>0</v>
       </c>
       <c r="B33">
-        <v>1329500</v>
+        <v>1329490</v>
       </c>
       <c r="C33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1021,10 +1018,10 @@
         <v>0</v>
       </c>
       <c r="B34">
-        <v>1330000</v>
+        <v>1329500</v>
       </c>
       <c r="C34" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1032,10 +1029,10 @@
         <v>0</v>
       </c>
       <c r="B35">
-        <v>1330500</v>
+        <v>1330000</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1043,10 +1040,10 @@
         <v>0</v>
       </c>
       <c r="B36">
-        <v>1334500</v>
+        <v>1330500</v>
       </c>
       <c r="C36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1054,10 +1051,10 @@
         <v>0</v>
       </c>
       <c r="B37">
-        <v>1335754</v>
+        <v>1334500</v>
       </c>
       <c r="C37" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1065,10 +1062,10 @@
         <v>0</v>
       </c>
       <c r="B38">
-        <v>1335755</v>
+        <v>1335754</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1076,39 +1073,39 @@
         <v>0</v>
       </c>
       <c r="B39">
+        <v>1335755</v>
+      </c>
+      <c r="C39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40">
         <v>1358000</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-    </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41">
-        <v>1359133</v>
-      </c>
-      <c r="C41" t="s">
-        <v>33</v>
-      </c>
+      <c r="A41" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>0</v>
       </c>
       <c r="B42">
-        <v>1359135</v>
+        <v>1359133</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1116,10 +1113,10 @@
         <v>0</v>
       </c>
       <c r="B43">
-        <v>1359528</v>
+        <v>1359135</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1127,10 +1124,10 @@
         <v>0</v>
       </c>
       <c r="B44">
-        <v>1359750</v>
+        <v>1359528</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1138,10 +1135,10 @@
         <v>0</v>
       </c>
       <c r="B45">
-        <v>1360640</v>
+        <v>1359750</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1149,10 +1146,10 @@
         <v>0</v>
       </c>
       <c r="B46">
-        <v>1361000</v>
+        <v>1360640</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1160,10 +1157,10 @@
         <v>0</v>
       </c>
       <c r="B47">
-        <v>1361200</v>
+        <v>1361000</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1171,10 +1168,10 @@
         <v>0</v>
       </c>
       <c r="B48">
-        <v>1362090</v>
+        <v>1361200</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1182,10 +1179,10 @@
         <v>0</v>
       </c>
       <c r="B49">
-        <v>1362192</v>
+        <v>1362090</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1193,10 +1190,10 @@
         <v>0</v>
       </c>
       <c r="B50">
-        <v>136219503</v>
+        <v>1362192</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1204,10 +1201,10 @@
         <v>0</v>
       </c>
       <c r="B51">
-        <v>13621955</v>
+        <v>136219503</v>
       </c>
       <c r="C51" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1215,10 +1212,10 @@
         <v>0</v>
       </c>
       <c r="B52">
-        <v>1362200</v>
+        <v>13621955</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1226,10 +1223,10 @@
         <v>0</v>
       </c>
       <c r="B53">
-        <v>1362230</v>
+        <v>1362200</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1237,10 +1234,10 @@
         <v>0</v>
       </c>
       <c r="B54">
-        <v>1362297</v>
+        <v>1362230</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1248,10 +1245,10 @@
         <v>0</v>
       </c>
       <c r="B55">
-        <v>136230002</v>
+        <v>1362297</v>
       </c>
       <c r="C55" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1259,10 +1256,10 @@
         <v>0</v>
       </c>
       <c r="B56">
-        <v>1362322</v>
+        <v>136230002</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1270,10 +1267,10 @@
         <v>0</v>
       </c>
       <c r="B57">
-        <v>1362336</v>
+        <v>1362322</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1281,10 +1278,10 @@
         <v>0</v>
       </c>
       <c r="B58">
-        <v>1362342</v>
+        <v>1362336</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1292,10 +1289,10 @@
         <v>0</v>
       </c>
       <c r="B59">
-        <v>1362357</v>
+        <v>1362342</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1303,10 +1300,10 @@
         <v>0</v>
       </c>
       <c r="B60">
-        <v>1362368</v>
+        <v>1362357</v>
       </c>
       <c r="C60" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1314,10 +1311,10 @@
         <v>0</v>
       </c>
       <c r="B61">
-        <v>1362370</v>
+        <v>1362368</v>
       </c>
       <c r="C61" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1325,10 +1322,10 @@
         <v>0</v>
       </c>
       <c r="B62">
-        <v>1362380</v>
+        <v>1362370</v>
       </c>
       <c r="C62" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1336,10 +1333,10 @@
         <v>0</v>
       </c>
       <c r="B63">
-        <v>1362465</v>
+        <v>1362380</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1347,10 +1344,10 @@
         <v>0</v>
       </c>
       <c r="B64">
-        <v>1362487</v>
+        <v>1362465</v>
       </c>
       <c r="C64" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1358,10 +1355,10 @@
         <v>0</v>
       </c>
       <c r="B65">
-        <v>1362497</v>
+        <v>1362487</v>
       </c>
       <c r="C65" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1369,10 +1366,10 @@
         <v>0</v>
       </c>
       <c r="B66">
-        <v>1362500</v>
+        <v>1362497</v>
       </c>
       <c r="C66" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1380,10 +1377,10 @@
         <v>0</v>
       </c>
       <c r="B67">
-        <v>1363382</v>
+        <v>1362500</v>
       </c>
       <c r="C67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1391,10 +1388,10 @@
         <v>0</v>
       </c>
       <c r="B68">
-        <v>1363556</v>
+        <v>1363382</v>
       </c>
       <c r="C68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1402,68 +1399,68 @@
         <v>0</v>
       </c>
       <c r="B69">
+        <v>1363556</v>
+      </c>
+      <c r="C69" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B70">
         <v>1364500</v>
       </c>
-      <c r="C69" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B70" s="1"/>
-      <c r="C70" s="1"/>
+      <c r="C70" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B71">
-        <v>1372051</v>
-      </c>
-      <c r="C71" t="s">
-        <v>62</v>
-      </c>
+      <c r="A71" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>0</v>
       </c>
       <c r="B72">
+        <v>1372051</v>
+      </c>
+      <c r="C72" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>0</v>
+      </c>
+      <c r="B73">
         <v>1372500</v>
       </c>
-      <c r="C72" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B73" s="1"/>
-      <c r="C73" s="1"/>
+      <c r="C73" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>0</v>
-      </c>
-      <c r="B74">
-        <v>137449480</v>
-      </c>
-      <c r="C74" t="s">
-        <v>66</v>
-      </c>
+      <c r="A74" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>0</v>
       </c>
       <c r="B75">
-        <v>1374505</v>
+        <v>137449480</v>
       </c>
       <c r="C75" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
@@ -1471,10 +1468,10 @@
         <v>0</v>
       </c>
       <c r="B76">
-        <v>1374531</v>
+        <v>1374505</v>
       </c>
       <c r="C76" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
@@ -1482,10 +1479,10 @@
         <v>0</v>
       </c>
       <c r="B77">
-        <v>1374559</v>
+        <v>1374531</v>
       </c>
       <c r="C77" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
@@ -1493,10 +1490,10 @@
         <v>0</v>
       </c>
       <c r="B78">
-        <v>1374581</v>
+        <v>1374559</v>
       </c>
       <c r="C78" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
@@ -1504,10 +1501,10 @@
         <v>0</v>
       </c>
       <c r="B79">
-        <v>1374598</v>
+        <v>1374581</v>
       </c>
       <c r="C79" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
@@ -1515,10 +1512,10 @@
         <v>0</v>
       </c>
       <c r="B80">
-        <v>137462010</v>
+        <v>1374598</v>
       </c>
       <c r="C80" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
@@ -1526,10 +1523,10 @@
         <v>0</v>
       </c>
       <c r="B81">
-        <v>1374654</v>
+        <v>137462010</v>
       </c>
       <c r="C81" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
@@ -1537,10 +1534,10 @@
         <v>0</v>
       </c>
       <c r="B82">
-        <v>1374701</v>
+        <v>1374654</v>
       </c>
       <c r="C82" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
@@ -1548,10 +1545,10 @@
         <v>0</v>
       </c>
       <c r="B83">
-        <v>1374781</v>
+        <v>1374701</v>
       </c>
       <c r="C83" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
@@ -1559,10 +1556,10 @@
         <v>0</v>
       </c>
       <c r="B84">
-        <v>1374821</v>
+        <v>1374781</v>
       </c>
       <c r="C84" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
@@ -1570,10 +1567,10 @@
         <v>0</v>
       </c>
       <c r="B85">
-        <v>1374890</v>
+        <v>1374821</v>
       </c>
       <c r="C85" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
@@ -1581,10 +1578,10 @@
         <v>0</v>
       </c>
       <c r="B86">
-        <v>1374901</v>
+        <v>1374890</v>
       </c>
       <c r="C86" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
@@ -1592,10 +1589,10 @@
         <v>0</v>
       </c>
       <c r="B87">
-        <v>1374918</v>
+        <v>1374901</v>
       </c>
       <c r="C87" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
@@ -1603,10 +1600,10 @@
         <v>0</v>
       </c>
       <c r="B88">
-        <v>1374930</v>
+        <v>1374918</v>
       </c>
       <c r="C88" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
@@ -1614,10 +1611,10 @@
         <v>0</v>
       </c>
       <c r="B89">
-        <v>1374941</v>
+        <v>1374930</v>
       </c>
       <c r="C89" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
@@ -1625,10 +1622,10 @@
         <v>0</v>
       </c>
       <c r="B90">
-        <v>1374976</v>
+        <v>1374941</v>
       </c>
       <c r="C90" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
@@ -1636,10 +1633,10 @@
         <v>0</v>
       </c>
       <c r="B91">
-        <v>1374987</v>
+        <v>1374976</v>
       </c>
       <c r="C91" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
@@ -1647,10 +1644,10 @@
         <v>0</v>
       </c>
       <c r="B92">
-        <v>137499350</v>
+        <v>1374987</v>
       </c>
       <c r="C92" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
@@ -1658,89 +1655,100 @@
         <v>0</v>
       </c>
       <c r="B93">
+        <v>137499350</v>
+      </c>
+      <c r="C93" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>0</v>
+      </c>
+      <c r="B94">
         <v>1375000</v>
       </c>
-      <c r="C93" t="s">
-        <v>85</v>
+      <c r="C94" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A29:C29"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="A74:C74"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01312000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{11ED6669-AD84-4CC4-8A65-F4E816A8CCE2}"/>
-    <hyperlink ref="B2" r:id="rId2" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{0EDDEE4B-56A4-42FE-89D0-E0070B25EF0A}"/>
-    <hyperlink ref="B3" r:id="rId3" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01318500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{72BD276E-CD6F-46CC-900F-90BB9631FAF5}"/>
-    <hyperlink ref="B4" r:id="rId4" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01327750&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DA7C56A9-C174-40D7-9535-876FD24C4C91}"/>
-    <hyperlink ref="B5" r:id="rId5" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01328770&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{3AE84601-B8EF-44D0-9A3C-7F3288AE928D}"/>
-    <hyperlink ref="B6" r:id="rId6" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335754&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{C1255E7E-0D21-4ED7-BC08-E1A965369A1D}"/>
-    <hyperlink ref="B7" r:id="rId7" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335755&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{2D39DB6E-A2C9-4441-AE2B-E1E91DCAB286}"/>
-    <hyperlink ref="B8" r:id="rId8" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01358000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{F86510B8-8486-4190-8243-CFD7E9185CE5}"/>
-    <hyperlink ref="B9" r:id="rId9" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359139&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{97F71F9A-ADCE-44AF-83EA-B68C270CE629}"/>
-    <hyperlink ref="B10" r:id="rId10" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359165&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{534C4F9A-4163-4AD8-B48E-78AF41981ACD}"/>
-    <hyperlink ref="B11" r:id="rId11" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0135980207&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{AB1F4388-12E3-46C6-AA52-815EFDCE85A1}"/>
-    <hyperlink ref="B12" r:id="rId12" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372043&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{1B04D761-EE25-4F63-816A-24979DCE307F}"/>
-    <hyperlink ref="B13" r:id="rId13" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372058&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{1B143E75-8E46-44E8-B7CB-2C566D1F4F63}"/>
-    <hyperlink ref="B14" r:id="rId14" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01374019&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{10F7AA30-E7B1-4309-A4C3-101D74A4E804}"/>
-    <hyperlink ref="B15" r:id="rId15" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376269&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{AE2FF8A6-2304-4FF2-AF21-44F3264201C3}"/>
-    <hyperlink ref="B16" r:id="rId16" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376307&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DD2A2061-00AA-4244-921F-DD96E40243C6}"/>
-    <hyperlink ref="B17" r:id="rId17" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376515&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B77952C8-F6FE-49F9-9AD4-2EC391B6AFA5}"/>
-    <hyperlink ref="B18" r:id="rId18" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376520&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{7C7E419D-9234-4CA0-9806-512077C45B76}"/>
-    <hyperlink ref="B27" r:id="rId19" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01318500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{38B2E3B5-37F2-41C2-8967-B5F60CDBFBB1}"/>
-    <hyperlink ref="B26" r:id="rId20" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{17F9BE5E-8219-44F5-ACBA-36CE64EA1607}"/>
-    <hyperlink ref="B25" r:id="rId21" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315227&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E4D5BBBD-0715-423E-994A-1093F5262902}"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315226&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DC44DCA7-DEE1-4FCC-9A65-905BFC6D9A19}"/>
-    <hyperlink ref="B23" r:id="rId23" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315170&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{9ED9FE18-504E-4248-AD19-80DFEE382CA5}"/>
-    <hyperlink ref="B22" r:id="rId24" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{40D48BA8-06B4-498D-AC48-69FA9CD73AC5}"/>
-    <hyperlink ref="B21" r:id="rId25" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01312000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{D4ACA5F1-DDD8-489B-A2CD-EF3267A2957E}"/>
-    <hyperlink ref="B20" r:id="rId26" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0131199050&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{181B2D68-6191-4484-B697-A725952ADB83}"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01327500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{75E42C80-0D13-432D-BA8F-41B135CE228A}"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01327750&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{85850217-81EE-4B0A-9D40-523E5FD4D001}"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01328770&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DEA1D2A5-B625-4E20-9FA0-163DA23E6410}"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01329490&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{26DE6BEB-AB09-4F32-9E3A-3D6DF0334D1B}"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01329500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{58379902-3EDB-45C3-AF31-924BBC8E6813}"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01330000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{19F81B5B-2E2B-4E5A-ADB1-B8A654D0CE96}"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01330500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{F6CC93AF-1831-42C5-9A81-65DE07348F7F}"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01334500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{6CE3D97F-889C-4A00-9E3D-C0FF06F11367}"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335754&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{A31852BF-E821-473E-B7B2-5451299E1CC1}"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335755&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{005CCADA-C5B1-4C56-BA8D-30E215C77174}"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01358000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{6FD6B712-6AA5-430D-B51A-ECB16B8FD3AE}"/>
-    <hyperlink ref="B41" r:id="rId38" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359133&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{679693FD-DDE5-4428-A273-9A3791F2D557}"/>
-    <hyperlink ref="B42" r:id="rId39" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359135&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B503CFDA-EB3E-4CED-B6ED-CCD12BB06F7E}"/>
-    <hyperlink ref="B43" r:id="rId40" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359528&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{9757E027-7648-4BF3-8EDA-BD7F89298DB3}"/>
-    <hyperlink ref="B44" r:id="rId41" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359750&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{4F157D21-C928-4E75-84B3-EAB58EA40BB1}"/>
-    <hyperlink ref="B45" r:id="rId42" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01360640&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{188694DF-FA25-4D54-92A0-4DB0ADD6C9BB}"/>
-    <hyperlink ref="B46" r:id="rId43" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01361000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{457BC2D4-2DE3-4E4C-9AE3-36D6E2E7DD6F}"/>
-    <hyperlink ref="B47" r:id="rId44" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01361200&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{64385F62-746B-489D-AD64-32990E5E4576}"/>
-    <hyperlink ref="B48" r:id="rId45" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362090&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{78BF616A-EEC2-4EDF-A933-50D989104417}"/>
-    <hyperlink ref="B49" r:id="rId46" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362192&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{8A2740C0-609A-46A7-971E-854CD19B2B4D}"/>
-    <hyperlink ref="B50" r:id="rId47" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0136219503&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E9B5A534-4ED6-49D1-8BBF-17B6C0063D8D}"/>
-    <hyperlink ref="B51" r:id="rId48" display="https://waterdata.usgs.gov/nwis/uv/?site_no=013621955&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{FA5FC687-A787-46EB-BD03-364F7E2321F0}"/>
-    <hyperlink ref="B52" r:id="rId49" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362200&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{65D9BC90-3376-4E92-AA1B-70981C9DE40B}"/>
-    <hyperlink ref="B53" r:id="rId50" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362230&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DE18BA4F-0264-41C8-A6A9-4B95A92D9BEF}"/>
-    <hyperlink ref="B54" r:id="rId51" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362297&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E8807314-53D3-4CC2-AA9D-C9F5A0494D33}"/>
-    <hyperlink ref="B55" r:id="rId52" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0136230002&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{A7B2AD99-71D9-4F14-984E-578FA6680FE9}"/>
-    <hyperlink ref="B56" r:id="rId53" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362322&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{CB696C9E-B5F1-4DF6-987B-A28458880BEE}"/>
-    <hyperlink ref="B57" r:id="rId54" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362336&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{FA78778C-E18D-44B2-A9B7-00AE80DF08BD}"/>
-    <hyperlink ref="B58" r:id="rId55" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362342&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{5FA10C7C-F0E0-4C82-80A8-BD9453D34DCF}"/>
-    <hyperlink ref="B59" r:id="rId56" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362357&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{10B568C1-6305-4779-843A-433F18D562AA}"/>
-    <hyperlink ref="B60" r:id="rId57" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362368&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B9B5005B-34CD-4CBB-AD48-6E055B7DE382}"/>
-    <hyperlink ref="B61" r:id="rId58" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362370&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{5655F6B8-325C-4DBA-9AAE-22C6802CE4CA}"/>
-    <hyperlink ref="B62" r:id="rId59" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362380&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{94855F01-BF54-4269-8DE4-7B7D256F154C}"/>
-    <hyperlink ref="B63" r:id="rId60" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362465&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B7BA992F-0DF2-4657-8631-684CE9969186}"/>
-    <hyperlink ref="B64" r:id="rId61" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362487&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{7BA8CB9D-1ED0-4CB2-A74E-101DC0225409}"/>
-    <hyperlink ref="B65" r:id="rId62" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362497&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{BBC59CEF-7908-41BB-A5AE-765A746ACDF3}"/>
-    <hyperlink ref="B66" r:id="rId63" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{6D18A2DC-9B5B-4FC0-A171-4C0E73B6E623}"/>
-    <hyperlink ref="B67" r:id="rId64" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01363382&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{3A4631B0-DEF5-4526-9F3D-32B38C3B5F2A}"/>
-    <hyperlink ref="B68" r:id="rId65" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01363556&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{047D375B-09B9-4981-8213-EA1F42090A21}"/>
-    <hyperlink ref="B69" r:id="rId66" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01364500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{222C4DB8-DC9B-45EF-85BD-F04796D56C80}"/>
-    <hyperlink ref="B71" r:id="rId67" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372051&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E66A56A2-2180-4897-8ED2-D7F610D0D28D}"/>
-    <hyperlink ref="B72" r:id="rId68" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{17DA8902-9469-443A-B5D9-A7C162F6444A}"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01312000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{11ED6669-AD84-4CC4-8A65-F4E816A8CCE2}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{0EDDEE4B-56A4-42FE-89D0-E0070B25EF0A}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01318500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{72BD276E-CD6F-46CC-900F-90BB9631FAF5}"/>
+    <hyperlink ref="B5" r:id="rId4" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01327750&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DA7C56A9-C174-40D7-9535-876FD24C4C91}"/>
+    <hyperlink ref="B6" r:id="rId5" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01328770&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{3AE84601-B8EF-44D0-9A3C-7F3288AE928D}"/>
+    <hyperlink ref="B7" r:id="rId6" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335754&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{C1255E7E-0D21-4ED7-BC08-E1A965369A1D}"/>
+    <hyperlink ref="B8" r:id="rId7" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335755&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{2D39DB6E-A2C9-4441-AE2B-E1E91DCAB286}"/>
+    <hyperlink ref="B9" r:id="rId8" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01358000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{F86510B8-8486-4190-8243-CFD7E9185CE5}"/>
+    <hyperlink ref="B10" r:id="rId9" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359139&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{97F71F9A-ADCE-44AF-83EA-B68C270CE629}"/>
+    <hyperlink ref="B11" r:id="rId10" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359165&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{534C4F9A-4163-4AD8-B48E-78AF41981ACD}"/>
+    <hyperlink ref="B12" r:id="rId11" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0135980207&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{AB1F4388-12E3-46C6-AA52-815EFDCE85A1}"/>
+    <hyperlink ref="B13" r:id="rId12" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372043&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{1B04D761-EE25-4F63-816A-24979DCE307F}"/>
+    <hyperlink ref="B14" r:id="rId13" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372058&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{1B143E75-8E46-44E8-B7CB-2C566D1F4F63}"/>
+    <hyperlink ref="B15" r:id="rId14" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01374019&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{10F7AA30-E7B1-4309-A4C3-101D74A4E804}"/>
+    <hyperlink ref="B16" r:id="rId15" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376269&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{AE2FF8A6-2304-4FF2-AF21-44F3264201C3}"/>
+    <hyperlink ref="B17" r:id="rId16" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376307&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DD2A2061-00AA-4244-921F-DD96E40243C6}"/>
+    <hyperlink ref="B18" r:id="rId17" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376515&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B77952C8-F6FE-49F9-9AD4-2EC391B6AFA5}"/>
+    <hyperlink ref="B19" r:id="rId18" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01376520&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{7C7E419D-9234-4CA0-9806-512077C45B76}"/>
+    <hyperlink ref="B28" r:id="rId19" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01318500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{38B2E3B5-37F2-41C2-8967-B5F60CDBFBB1}"/>
+    <hyperlink ref="B27" r:id="rId20" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{17F9BE5E-8219-44F5-ACBA-36CE64EA1607}"/>
+    <hyperlink ref="B26" r:id="rId21" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315227&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E4D5BBBD-0715-423E-994A-1093F5262902}"/>
+    <hyperlink ref="B25" r:id="rId22" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315226&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DC44DCA7-DEE1-4FCC-9A65-905BFC6D9A19}"/>
+    <hyperlink ref="B24" r:id="rId23" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315170&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{9ED9FE18-504E-4248-AD19-80DFEE382CA5}"/>
+    <hyperlink ref="B23" r:id="rId24" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01315000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{40D48BA8-06B4-498D-AC48-69FA9CD73AC5}"/>
+    <hyperlink ref="B22" r:id="rId25" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01312000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{D4ACA5F1-DDD8-489B-A2CD-EF3267A2957E}"/>
+    <hyperlink ref="B21" r:id="rId26" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0131199050&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{181B2D68-6191-4484-B697-A725952ADB83}"/>
+    <hyperlink ref="B30" r:id="rId27" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01327500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{75E42C80-0D13-432D-BA8F-41B135CE228A}"/>
+    <hyperlink ref="B31" r:id="rId28" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01327750&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{85850217-81EE-4B0A-9D40-523E5FD4D001}"/>
+    <hyperlink ref="B32" r:id="rId29" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01328770&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DEA1D2A5-B625-4E20-9FA0-163DA23E6410}"/>
+    <hyperlink ref="B33" r:id="rId30" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01329490&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{26DE6BEB-AB09-4F32-9E3A-3D6DF0334D1B}"/>
+    <hyperlink ref="B34" r:id="rId31" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01329500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{58379902-3EDB-45C3-AF31-924BBC8E6813}"/>
+    <hyperlink ref="B35" r:id="rId32" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01330000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{19F81B5B-2E2B-4E5A-ADB1-B8A654D0CE96}"/>
+    <hyperlink ref="B36" r:id="rId33" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01330500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{F6CC93AF-1831-42C5-9A81-65DE07348F7F}"/>
+    <hyperlink ref="B37" r:id="rId34" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01334500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{6CE3D97F-889C-4A00-9E3D-C0FF06F11367}"/>
+    <hyperlink ref="B38" r:id="rId35" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335754&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{A31852BF-E821-473E-B7B2-5451299E1CC1}"/>
+    <hyperlink ref="B39" r:id="rId36" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01335755&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{005CCADA-C5B1-4C56-BA8D-30E215C77174}"/>
+    <hyperlink ref="B40" r:id="rId37" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01358000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{6FD6B712-6AA5-430D-B51A-ECB16B8FD3AE}"/>
+    <hyperlink ref="B42" r:id="rId38" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359133&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{679693FD-DDE5-4428-A273-9A3791F2D557}"/>
+    <hyperlink ref="B43" r:id="rId39" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359135&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B503CFDA-EB3E-4CED-B6ED-CCD12BB06F7E}"/>
+    <hyperlink ref="B44" r:id="rId40" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359528&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{9757E027-7648-4BF3-8EDA-BD7F89298DB3}"/>
+    <hyperlink ref="B45" r:id="rId41" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01359750&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{4F157D21-C928-4E75-84B3-EAB58EA40BB1}"/>
+    <hyperlink ref="B46" r:id="rId42" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01360640&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{188694DF-FA25-4D54-92A0-4DB0ADD6C9BB}"/>
+    <hyperlink ref="B47" r:id="rId43" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01361000&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{457BC2D4-2DE3-4E4C-9AE3-36D6E2E7DD6F}"/>
+    <hyperlink ref="B48" r:id="rId44" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01361200&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{64385F62-746B-489D-AD64-32990E5E4576}"/>
+    <hyperlink ref="B49" r:id="rId45" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362090&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{78BF616A-EEC2-4EDF-A933-50D989104417}"/>
+    <hyperlink ref="B50" r:id="rId46" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362192&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{8A2740C0-609A-46A7-971E-854CD19B2B4D}"/>
+    <hyperlink ref="B51" r:id="rId47" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0136219503&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E9B5A534-4ED6-49D1-8BBF-17B6C0063D8D}"/>
+    <hyperlink ref="B52" r:id="rId48" display="https://waterdata.usgs.gov/nwis/uv/?site_no=013621955&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{FA5FC687-A787-46EB-BD03-364F7E2321F0}"/>
+    <hyperlink ref="B53" r:id="rId49" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362200&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{65D9BC90-3376-4E92-AA1B-70981C9DE40B}"/>
+    <hyperlink ref="B54" r:id="rId50" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362230&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{DE18BA4F-0264-41C8-A6A9-4B95A92D9BEF}"/>
+    <hyperlink ref="B55" r:id="rId51" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362297&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E8807314-53D3-4CC2-AA9D-C9F5A0494D33}"/>
+    <hyperlink ref="B56" r:id="rId52" display="https://waterdata.usgs.gov/nwis/uv/?site_no=0136230002&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{A7B2AD99-71D9-4F14-984E-578FA6680FE9}"/>
+    <hyperlink ref="B57" r:id="rId53" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362322&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{CB696C9E-B5F1-4DF6-987B-A28458880BEE}"/>
+    <hyperlink ref="B58" r:id="rId54" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362336&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{FA78778C-E18D-44B2-A9B7-00AE80DF08BD}"/>
+    <hyperlink ref="B59" r:id="rId55" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362342&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{5FA10C7C-F0E0-4C82-80A8-BD9453D34DCF}"/>
+    <hyperlink ref="B60" r:id="rId56" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362357&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{10B568C1-6305-4779-843A-433F18D562AA}"/>
+    <hyperlink ref="B61" r:id="rId57" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362368&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B9B5005B-34CD-4CBB-AD48-6E055B7DE382}"/>
+    <hyperlink ref="B62" r:id="rId58" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362370&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{5655F6B8-325C-4DBA-9AAE-22C6802CE4CA}"/>
+    <hyperlink ref="B63" r:id="rId59" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362380&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{94855F01-BF54-4269-8DE4-7B7D256F154C}"/>
+    <hyperlink ref="B64" r:id="rId60" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362465&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{B7BA992F-0DF2-4657-8631-684CE9969186}"/>
+    <hyperlink ref="B65" r:id="rId61" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362487&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{7BA8CB9D-1ED0-4CB2-A74E-101DC0225409}"/>
+    <hyperlink ref="B66" r:id="rId62" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362497&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{BBC59CEF-7908-41BB-A5AE-765A746ACDF3}"/>
+    <hyperlink ref="B67" r:id="rId63" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01362500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{6D18A2DC-9B5B-4FC0-A171-4C0E73B6E623}"/>
+    <hyperlink ref="B68" r:id="rId64" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01363382&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{3A4631B0-DEF5-4526-9F3D-32B38C3B5F2A}"/>
+    <hyperlink ref="B69" r:id="rId65" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01363556&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{047D375B-09B9-4981-8213-EA1F42090A21}"/>
+    <hyperlink ref="B70" r:id="rId66" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01364500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{222C4DB8-DC9B-45EF-85BD-F04796D56C80}"/>
+    <hyperlink ref="B72" r:id="rId67" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372051&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{E66A56A2-2180-4897-8ED2-D7F610D0D28D}"/>
+    <hyperlink ref="B73" r:id="rId68" display="https://waterdata.usgs.gov/nwis/uv/?site_no=01372500&amp;agency_cd=USGS&amp;amp;referred_module=sw" xr:uid="{17DA8902-9469-443A-B5D9-A7C162F6444A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId69"/>

</xml_diff>